<commit_message>
Fix issue with reading PDF from FHI
</commit_message>
<xml_diff>
--- a/data/04_deaths/deaths_total_fhi.xlsx
+++ b/data/04_deaths/deaths_total_fhi.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -380,365 +380,420 @@
       <c r="A2" s="2">
         <v>43940</v>
       </c>
-      <c r="B2">
-        <v>104</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 154</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>43940</v>
-      </c>
-      <c r="B3">
-        <v>154</v>
+        <v>43939</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 148</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>43939</v>
-      </c>
-      <c r="B4">
-        <v>962</v>
+        <v>43938</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 137</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>43939</v>
-      </c>
-      <c r="B5">
-        <v>148</v>
+        <v>43937</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 136</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>43938</v>
-      </c>
-      <c r="B6">
-        <v>873</v>
+        <v>43936</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 130</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>43938</v>
-      </c>
-      <c r="B7">
-        <v>137</v>
+        <v>43935</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 127</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>43937</v>
-      </c>
-      <c r="B8">
-        <v>136</v>
+        <v>43934</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 114</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>43936</v>
-      </c>
-      <c r="B9">
-        <v>130</v>
+        <v>43933</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 103</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>43935</v>
-      </c>
-      <c r="B10">
-        <v>127</v>
+        <v>43932</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 98</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>43934</v>
-      </c>
-      <c r="B11">
-        <v>114</v>
+        <v>43931</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 92</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>43933</v>
-      </c>
-      <c r="B12">
-        <v>103</v>
+        <v>43930</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 88</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>43932</v>
-      </c>
-      <c r="B13">
-        <v>98</v>
+        <v>43929</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 80</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>43931</v>
-      </c>
-      <c r="B14">
-        <v>92</v>
+        <v>43928</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 69</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>43930</v>
-      </c>
-      <c r="B15">
-        <v>88</v>
+        <v>43927</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 59</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>43929</v>
-      </c>
-      <c r="B16">
-        <v>80</v>
+        <v>43926</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 58</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>43928</v>
-      </c>
-      <c r="B17">
-        <v>69</v>
+        <v>43925</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 50</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>43927</v>
-      </c>
-      <c r="B18">
-        <v>59</v>
+        <v>43924</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 44</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>43926</v>
-      </c>
-      <c r="B19">
-        <v>58</v>
+        <v>43923</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 42</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>43925</v>
-      </c>
-      <c r="B20">
-        <v>50</v>
+        <v>43922</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 32</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>43924</v>
-      </c>
-      <c r="B21">
-        <v>44</v>
+        <v>43921</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>43923</v>
-      </c>
-      <c r="B22">
-        <v>42</v>
+        <v>43920</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>43922</v>
-      </c>
-      <c r="B23">
-        <v>32</v>
+        <v>43919</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 22</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>43921</v>
-      </c>
-      <c r="B24">
-        <v>28</v>
+        <v>43918</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>43920</v>
-      </c>
-      <c r="B25">
-        <v>26</v>
+        <v>43917</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>43919</v>
-      </c>
-      <c r="B26">
-        <v>22</v>
+        <v>43916</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>43918</v>
-      </c>
-      <c r="B27">
-        <v>20</v>
+        <v>43915</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>43917</v>
-      </c>
-      <c r="B28">
-        <v>16</v>
+        <v>43914</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>43916</v>
-      </c>
-      <c r="B29">
-        <v>14</v>
+        <v>43913</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>43915</v>
-      </c>
-      <c r="B30">
-        <v>12</v>
+        <v>43912</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>43914</v>
-      </c>
-      <c r="B31">
-        <v>10</v>
+        <v>43911</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>43913</v>
-      </c>
-      <c r="B32">
-        <v>8</v>
+        <v>43910</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>43912</v>
-      </c>
-      <c r="B33">
-        <v>7</v>
+        <v>43909</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>43911</v>
-      </c>
-      <c r="B34">
-        <v>7</v>
+        <v>43908</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>43910</v>
-      </c>
-      <c r="B35">
-        <v>7</v>
+        <v>43907</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>43909</v>
-      </c>
-      <c r="B36">
-        <v>6</v>
+        <v>43906</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>43908</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
+        <v>43905</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>43907</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
+        <v>43904</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>43906</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
+        <v>43903</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>43905</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
+        <v>43902</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>43904</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
+        <v>43901</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>43903</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
+        <v>43900</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>43902</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2">
-        <v>43901</v>
-      </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2">
-        <v>43900</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2">
         <v>43899</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47">
-        <v>722</v>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>